<commit_message>
Update Data Team Version IDIS Team Formation.xlsx
</commit_message>
<xml_diff>
--- a/Data Team Version IDIS Team Formation.xlsx
+++ b/Data Team Version IDIS Team Formation.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iveyca-my.sharepoint.com/personal/scortez_msc2021_ivey_ca/Documents/Third Term/Ivey Digital lab/Team Formation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocks\Documents\GitHub\Team-Formation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{D55D8C52-B675-4507-8841-6F9D90F2C0DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9FF23995-928C-BE41-ABEC-D4BD3EAD359F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5EC32E-51C6-4D52-B932-70DEEE4598D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forwarded to Team" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="34">
   <si>
     <t>Liberal Arts</t>
   </si>
@@ -116,6 +127,12 @@
   </si>
   <si>
     <t>5&amp;32</t>
+  </si>
+  <si>
+    <t>Priority Preference</t>
+  </si>
+  <si>
+    <t>Priority preference</t>
   </si>
 </sst>
 </file>
@@ -549,25 +566,25 @@
   <dimension ref="A1:Z56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" customWidth="1"/>
-    <col min="21" max="21" width="11.5" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" customWidth="1"/>
-    <col min="24" max="25" width="17.1640625" customWidth="1"/>
-    <col min="26" max="26" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="8.36328125" customWidth="1"/>
+    <col min="3" max="4" width="12.6328125" customWidth="1"/>
+    <col min="21" max="21" width="11.453125" customWidth="1"/>
+    <col min="22" max="22" width="12.1796875" customWidth="1"/>
+    <col min="23" max="23" width="16.6328125" customWidth="1"/>
+    <col min="24" max="25" width="17.1796875" customWidth="1"/>
+    <col min="26" max="26" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="105" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="98" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -634,12 +651,14 @@
       <c r="V1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="2"/>
+      <c r="W1" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -662,7 +681,7 @@
       <c r="W2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>27</v>
       </c>
@@ -683,7 +702,7 @@
       <c r="W3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -705,10 +724,12 @@
       <c r="U4" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="1"/>
+      <c r="W4" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>32</v>
       </c>
@@ -731,7 +752,7 @@
       <c r="W5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>29</v>
       </c>
@@ -752,7 +773,7 @@
       <c r="W6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>41</v>
       </c>
@@ -777,7 +798,7 @@
       <c r="W7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>24</v>
       </c>
@@ -799,10 +820,12 @@
       <c r="U8" t="s">
         <v>16</v>
       </c>
-      <c r="W8" s="1"/>
+      <c r="W8" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -824,10 +847,12 @@
       <c r="U9" t="s">
         <v>16</v>
       </c>
-      <c r="W9" s="1"/>
+      <c r="W9" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>31</v>
       </c>
@@ -850,7 +875,7 @@
       <c r="W10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>28</v>
       </c>
@@ -875,7 +900,7 @@
       <c r="W11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>26</v>
       </c>
@@ -900,7 +925,7 @@
       <c r="W12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>43</v>
       </c>
@@ -925,7 +950,7 @@
       <c r="W13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>47</v>
       </c>
@@ -950,7 +975,7 @@
       <c r="W14" s="1"/>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -972,10 +997,12 @@
       <c r="U15" t="s">
         <v>16</v>
       </c>
-      <c r="W15" s="1"/>
+      <c r="W15" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>17</v>
       </c>
@@ -996,7 +1023,7 @@
       <c r="W16" s="1"/>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>34</v>
       </c>
@@ -1021,7 +1048,7 @@
       <c r="W17" s="1"/>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -1046,7 +1073,7 @@
       <c r="W18" s="1"/>
       <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>39</v>
       </c>
@@ -1069,7 +1096,7 @@
       <c r="W19" s="1"/>
       <c r="Y19" s="1"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>23</v>
       </c>
@@ -1094,7 +1121,7 @@
       <c r="W20" s="1"/>
       <c r="Y20" s="1"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>33</v>
       </c>
@@ -1119,7 +1146,7 @@
       <c r="W21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>3</v>
       </c>
@@ -1142,7 +1169,7 @@
       <c r="W22" s="1"/>
       <c r="Y22" s="1"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>13</v>
       </c>
@@ -1163,7 +1190,7 @@
       <c r="W23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>35</v>
       </c>
@@ -1184,7 +1211,7 @@
       <c r="W24" s="1"/>
       <c r="Y24" s="1"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -1206,10 +1233,12 @@
       <c r="U25" t="s">
         <v>16</v>
       </c>
-      <c r="W25" s="1"/>
+      <c r="W25" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y25" s="1"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>16</v>
       </c>
@@ -1234,7 +1263,7 @@
       <c r="W26" s="1"/>
       <c r="Y26" s="1"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>38</v>
       </c>
@@ -1255,7 +1284,7 @@
       <c r="W27" s="1"/>
       <c r="Y27" s="1"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>44</v>
       </c>
@@ -1280,7 +1309,7 @@
       <c r="W28" s="1"/>
       <c r="Y28" s="1"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>10</v>
       </c>
@@ -1302,10 +1331,12 @@
       <c r="U29" t="s">
         <v>16</v>
       </c>
-      <c r="W29" s="1"/>
+      <c r="W29" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y29" s="1"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>20</v>
       </c>
@@ -1325,10 +1356,12 @@
       <c r="U30" t="s">
         <v>16</v>
       </c>
-      <c r="W30" s="1"/>
+      <c r="W30" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y30" s="1"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>40</v>
       </c>
@@ -1351,7 +1384,7 @@
       <c r="W31" s="1"/>
       <c r="Y31" s="1"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>12</v>
       </c>
@@ -1374,7 +1407,7 @@
       <c r="W32" s="1"/>
       <c r="Y32" s="1"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>14</v>
       </c>
@@ -1399,7 +1432,7 @@
       <c r="W33" s="1"/>
       <c r="Y33" s="1"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>7</v>
       </c>
@@ -1422,7 +1455,7 @@
       <c r="W34" s="1"/>
       <c r="Y34" s="1"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>9</v>
       </c>
@@ -1444,10 +1477,12 @@
       <c r="U35" t="s">
         <v>16</v>
       </c>
-      <c r="W35" s="1"/>
+      <c r="W35" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y35" s="1"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>19</v>
       </c>
@@ -1469,10 +1504,12 @@
       <c r="U36" t="s">
         <v>16</v>
       </c>
-      <c r="W36" s="1"/>
+      <c r="W36" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y36" s="1"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -1495,7 +1532,7 @@
       <c r="W37" s="1"/>
       <c r="Y37" s="1"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>22</v>
       </c>
@@ -1518,7 +1555,7 @@
       <c r="W38" s="1"/>
       <c r="Y38" s="1"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>45</v>
       </c>
@@ -1539,7 +1576,7 @@
       <c r="W39" s="1"/>
       <c r="Y39" s="1"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>36</v>
       </c>
@@ -1564,7 +1601,7 @@
       <c r="W40" s="1"/>
       <c r="Y40" s="1"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>15</v>
       </c>
@@ -1586,10 +1623,12 @@
       <c r="U41" t="s">
         <v>16</v>
       </c>
-      <c r="W41" s="1"/>
+      <c r="W41" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y41" s="1"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>8</v>
       </c>
@@ -1610,7 +1649,7 @@
       <c r="W42" s="1"/>
       <c r="Y42" s="1"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>25</v>
       </c>
@@ -1630,10 +1669,12 @@
       <c r="U43" t="s">
         <v>16</v>
       </c>
-      <c r="W43" s="1"/>
+      <c r="W43" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y43" s="1"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>46</v>
       </c>
@@ -1658,7 +1699,7 @@
       <c r="W44" s="1"/>
       <c r="Y44" s="1"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>18</v>
       </c>
@@ -1683,7 +1724,7 @@
       <c r="W45" s="1"/>
       <c r="Y45" s="1"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -1705,10 +1746,12 @@
       <c r="U46" t="s">
         <v>16</v>
       </c>
-      <c r="W46" s="1"/>
+      <c r="W46" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Y46" s="1"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>30</v>
       </c>
@@ -1729,7 +1772,7 @@
       <c r="W47" s="1"/>
       <c r="Y47" s="1"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -1752,7 +1795,7 @@
       <c r="W48" s="1"/>
       <c r="Y48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>22</v>
       </c>
@@ -1762,7 +1805,7 @@
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>23</v>
       </c>
@@ -1772,7 +1815,7 @@
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>24</v>
       </c>
@@ -1782,7 +1825,7 @@
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>25</v>
       </c>
@@ -1792,7 +1835,7 @@
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>26</v>
       </c>
@@ -1802,7 +1845,7 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>27</v>
       </c>
@@ -1812,7 +1855,7 @@
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>28</v>
       </c>
@@ -1822,7 +1865,7 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>